<commit_message>
Add select ui Testinit java
</commit_message>
<xml_diff>
--- a/hybris-nao-tests/src/main/resources/BatchOrderUploadTest.xlsx
+++ b/hybris-nao-tests/src/main/resources/BatchOrderUploadTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\seleniumAutomationScripts\hybris\hyb4nov18\hybNov62017\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rajkumars\git\IRWWebservice\hybris-nao-tests\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C62BC9-21AB-456C-8C38-67467A3BB339}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9DDC82-440A-4801-B47C-04A74B43A539}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="19440" windowHeight="7470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="480" windowWidth="20460" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BatchOrderUploadTest" sheetId="18" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
   <si>
     <t>TestData2</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Bobcat of Regina, Ltd</t>
   </si>
   <si>
-    <t>Welcome@1</t>
-  </si>
-  <si>
     <t>TestData4</t>
   </si>
   <si>
@@ -124,12 +121,6 @@
     <t>A.C. McCartney Equipment, Inc., Carthage, IL</t>
   </si>
   <si>
-    <t>1364891</t>
-  </si>
-  <si>
-    <t>1364892</t>
-  </si>
-  <si>
     <t>1364893</t>
   </si>
   <si>
@@ -200,6 +191,24 @@
   </si>
   <si>
     <t>validFile</t>
+  </si>
+  <si>
+    <t>Welcome1</t>
+  </si>
+  <si>
+    <t>bobcat12</t>
+  </si>
+  <si>
+    <t>Bobcat12</t>
+  </si>
+  <si>
+    <t>1364907</t>
+  </si>
+  <si>
+    <t>1364909</t>
+  </si>
+  <si>
+    <t>1364910</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,37 +1203,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1241,25 +1250,25 @@
         <v>6</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>6</v>
@@ -1270,43 +1279,43 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="L3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1402,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6">
@@ -1406,25 +1415,25 @@
         <v>7</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>7</v>
@@ -1433,23 +1442,23 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
         <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I7" s="3">
         <v>7</v>
@@ -1471,13 +1480,13 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>2</v>
@@ -1489,10 +1498,10 @@
         <v>2</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K8" s="4">
         <v>110</v>
@@ -1506,13 +1515,13 @@
     </row>
     <row r="9" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>3</v>
@@ -1521,7 +1530,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>3</v>
@@ -1530,19 +1539,19 @@
         <v>3</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>3</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1559,25 +1568,25 @@
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="J10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>8</v>
@@ -1588,52 +1597,53 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="K11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="L11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="M11" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{8D423580-9759-4B45-BEC2-DB54A81633BE}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{40330722-6761-4AD3-A0F1-7C0F582EA107}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{4F087DFD-B7EB-456F-A031-DB448590DAE0}"/>
+    <hyperlink ref="A3" r:id="rId1" display="Welcome@1" xr:uid="{8D423580-9759-4B45-BEC2-DB54A81633BE}"/>
+    <hyperlink ref="B3" r:id="rId2" display="Welcome@1" xr:uid="{EE5E9D9F-E793-40CF-8EF2-07999F29C12B}"/>
+    <hyperlink ref="C3" r:id="rId3" display="Welcome@1" xr:uid="{B396FD8E-054B-4C24-B75A-E2FC24D4F18D}"/>
+    <hyperlink ref="D3" r:id="rId4" display="Welcome@1" xr:uid="{36239DA6-60D5-404B-82C4-3C7E459A96FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>